<commit_message>
Update Kendall tau values
</commit_message>
<xml_diff>
--- a/tables/Table_S3_predictors_of_assembly_quality.xlsx
+++ b/tables/Table_S3_predictors_of_assembly_quality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan/Dropbox/Uni_research/Projects/Polypolish_paper/GitHub_repo/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A08FBD6-85A9-9045-B9A3-66253A25B75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DB8C84-86F4-054C-9473-DDF0176E21C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2300" yWindow="-26700" windowWidth="35140" windowHeight="20400" xr2:uid="{7397BC90-3645-654F-B763-2CB018FF0480}"/>
   </bookViews>
@@ -616,21 +616,21 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,222 +962,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:104" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
-      <c r="AD1" s="20"/>
-      <c r="AE1" s="20"/>
-      <c r="AF1" s="20"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="20"/>
-      <c r="AL1" s="20"/>
-      <c r="AM1" s="20"/>
-      <c r="AN1" s="20"/>
-      <c r="AO1" s="20"/>
-      <c r="AP1" s="20"/>
-      <c r="AQ1" s="20"/>
-      <c r="AR1" s="20"/>
-      <c r="AS1" s="20"/>
-      <c r="AT1" s="20"/>
-      <c r="AU1" s="20"/>
-      <c r="AV1" s="20"/>
-      <c r="AW1" s="20"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="20"/>
-      <c r="BB1" s="20"/>
-      <c r="BC1" s="20"/>
-      <c r="BD1" s="20"/>
-      <c r="BE1" s="20"/>
-      <c r="BF1" s="20"/>
-      <c r="BG1" s="20"/>
-      <c r="BH1" s="20"/>
-      <c r="BI1" s="20"/>
-      <c r="BJ1" s="20"/>
-      <c r="BK1" s="20"/>
-      <c r="BL1" s="20"/>
-      <c r="BM1" s="20"/>
-      <c r="BN1" s="20"/>
-      <c r="BO1" s="20"/>
-      <c r="BP1" s="20"/>
-      <c r="BQ1" s="20"/>
-      <c r="BR1" s="20"/>
-      <c r="BS1" s="20"/>
-      <c r="BT1" s="20"/>
-      <c r="BU1" s="20"/>
-      <c r="BV1" s="20"/>
-      <c r="BW1" s="20"/>
-      <c r="BX1" s="20"/>
-      <c r="BY1" s="20"/>
-      <c r="BZ1" s="20"/>
-      <c r="CA1" s="20"/>
-      <c r="CB1" s="20"/>
-      <c r="CC1" s="20"/>
-      <c r="CD1" s="20"/>
-      <c r="CE1" s="20"/>
-      <c r="CF1" s="20"/>
-      <c r="CG1" s="20"/>
-      <c r="CH1" s="20"/>
-      <c r="CI1" s="20"/>
-      <c r="CJ1" s="20"/>
-      <c r="CK1" s="20"/>
-      <c r="CL1" s="20"/>
-      <c r="CM1" s="20"/>
-      <c r="CN1" s="20"/>
-      <c r="CO1" s="20"/>
-      <c r="CP1" s="20"/>
-      <c r="CQ1" s="20"/>
-      <c r="CR1" s="20"/>
-      <c r="CS1" s="20"/>
-      <c r="CT1" s="20"/>
-      <c r="CU1" s="20"/>
-      <c r="CV1" s="20"/>
-      <c r="CW1" s="20"/>
-      <c r="CX1" s="20"/>
-      <c r="CY1" s="20"/>
-      <c r="CZ1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
+      <c r="AN1" s="24"/>
+      <c r="AO1" s="24"/>
+      <c r="AP1" s="24"/>
+      <c r="AQ1" s="24"/>
+      <c r="AR1" s="24"/>
+      <c r="AS1" s="24"/>
+      <c r="AT1" s="24"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="24"/>
+      <c r="AW1" s="24"/>
+      <c r="AX1" s="24"/>
+      <c r="AY1" s="24"/>
+      <c r="AZ1" s="24"/>
+      <c r="BA1" s="24"/>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="24"/>
+      <c r="BF1" s="24"/>
+      <c r="BG1" s="24"/>
+      <c r="BH1" s="24"/>
+      <c r="BI1" s="24"/>
+      <c r="BJ1" s="24"/>
+      <c r="BK1" s="24"/>
+      <c r="BL1" s="24"/>
+      <c r="BM1" s="24"/>
+      <c r="BN1" s="24"/>
+      <c r="BO1" s="24"/>
+      <c r="BP1" s="24"/>
+      <c r="BQ1" s="24"/>
+      <c r="BR1" s="24"/>
+      <c r="BS1" s="24"/>
+      <c r="BT1" s="24"/>
+      <c r="BU1" s="24"/>
+      <c r="BV1" s="24"/>
+      <c r="BW1" s="24"/>
+      <c r="BX1" s="24"/>
+      <c r="BY1" s="24"/>
+      <c r="BZ1" s="24"/>
+      <c r="CA1" s="24"/>
+      <c r="CB1" s="24"/>
+      <c r="CC1" s="24"/>
+      <c r="CD1" s="24"/>
+      <c r="CE1" s="24"/>
+      <c r="CF1" s="24"/>
+      <c r="CG1" s="24"/>
+      <c r="CH1" s="24"/>
+      <c r="CI1" s="24"/>
+      <c r="CJ1" s="24"/>
+      <c r="CK1" s="24"/>
+      <c r="CL1" s="24"/>
+      <c r="CM1" s="24"/>
+      <c r="CN1" s="24"/>
+      <c r="CO1" s="24"/>
+      <c r="CP1" s="24"/>
+      <c r="CQ1" s="24"/>
+      <c r="CR1" s="24"/>
+      <c r="CS1" s="24"/>
+      <c r="CT1" s="24"/>
+      <c r="CU1" s="24"/>
+      <c r="CV1" s="24"/>
+      <c r="CW1" s="24"/>
+      <c r="CX1" s="24"/>
+      <c r="CY1" s="24"/>
+      <c r="CZ1" s="24"/>
     </row>
     <row r="2" spans="1:104" ht="19" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="T2" s="23"/>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="23"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="23"/>
-      <c r="AC2" s="23"/>
-      <c r="AD2" s="23"/>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="23"/>
-      <c r="AG2" s="23"/>
-      <c r="AH2" s="23"/>
-      <c r="AI2" s="23"/>
-      <c r="AJ2" s="23"/>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-      <c r="AR2" s="23"/>
-      <c r="AS2" s="23"/>
-      <c r="AT2" s="23"/>
-      <c r="AU2" s="23"/>
-      <c r="AV2" s="23"/>
-      <c r="AW2" s="23"/>
-      <c r="AX2" s="23"/>
-      <c r="AY2" s="23"/>
-      <c r="AZ2" s="23"/>
-      <c r="BA2" s="23"/>
-      <c r="BB2" s="23"/>
-      <c r="BC2" s="23"/>
-      <c r="BD2" s="23"/>
-      <c r="BE2" s="23"/>
-      <c r="BF2" s="23"/>
-      <c r="BG2" s="23"/>
-      <c r="BH2" s="23"/>
-      <c r="BI2" s="23"/>
-      <c r="BJ2" s="23"/>
-      <c r="BK2" s="23"/>
-      <c r="BL2" s="23"/>
-      <c r="BM2" s="23"/>
-      <c r="BN2" s="23"/>
-      <c r="BO2" s="23"/>
-      <c r="BP2" s="23"/>
-      <c r="BQ2" s="23"/>
-      <c r="BR2" s="23"/>
-      <c r="BS2" s="23"/>
-      <c r="BT2" s="23"/>
-      <c r="BU2" s="23"/>
-      <c r="BV2" s="23"/>
-      <c r="BW2" s="23"/>
-      <c r="BX2" s="23"/>
-      <c r="BY2" s="23"/>
-      <c r="BZ2" s="23"/>
-      <c r="CA2" s="23"/>
-      <c r="CB2" s="23"/>
-      <c r="CC2" s="23"/>
-      <c r="CD2" s="23"/>
-      <c r="CE2" s="23"/>
-      <c r="CF2" s="23"/>
-      <c r="CG2" s="23"/>
-      <c r="CH2" s="23"/>
-      <c r="CI2" s="23"/>
-      <c r="CJ2" s="23"/>
-      <c r="CK2" s="23"/>
-      <c r="CL2" s="23"/>
-      <c r="CM2" s="23"/>
-      <c r="CN2" s="23"/>
-      <c r="CO2" s="23"/>
-      <c r="CP2" s="23"/>
-      <c r="CQ2" s="23"/>
-      <c r="CR2" s="23"/>
-      <c r="CS2" s="23"/>
-      <c r="CT2" s="23"/>
-      <c r="CU2" s="23"/>
-      <c r="CV2" s="23"/>
-      <c r="CW2" s="23"/>
-      <c r="CX2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="22"/>
+      <c r="AI2" s="22"/>
+      <c r="AJ2" s="22"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+      <c r="AR2" s="22"/>
+      <c r="AS2" s="22"/>
+      <c r="AT2" s="22"/>
+      <c r="AU2" s="22"/>
+      <c r="AV2" s="22"/>
+      <c r="AW2" s="22"/>
+      <c r="AX2" s="22"/>
+      <c r="AY2" s="22"/>
+      <c r="AZ2" s="22"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22"/>
+      <c r="BE2" s="22"/>
+      <c r="BF2" s="22"/>
+      <c r="BG2" s="22"/>
+      <c r="BH2" s="22"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="22"/>
+      <c r="BR2" s="22"/>
+      <c r="BS2" s="22"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="22"/>
+      <c r="BY2" s="22"/>
+      <c r="BZ2" s="22"/>
+      <c r="CA2" s="22"/>
+      <c r="CB2" s="22"/>
+      <c r="CC2" s="22"/>
+      <c r="CD2" s="22"/>
+      <c r="CE2" s="22"/>
+      <c r="CF2" s="22"/>
+      <c r="CG2" s="22"/>
+      <c r="CH2" s="22"/>
+      <c r="CI2" s="22"/>
+      <c r="CJ2" s="22"/>
+      <c r="CK2" s="22"/>
+      <c r="CL2" s="22"/>
+      <c r="CM2" s="22"/>
+      <c r="CN2" s="22"/>
+      <c r="CO2" s="22"/>
+      <c r="CP2" s="22"/>
+      <c r="CQ2" s="22"/>
+      <c r="CR2" s="22"/>
+      <c r="CS2" s="22"/>
+      <c r="CT2" s="22"/>
+      <c r="CU2" s="22"/>
+      <c r="CV2" s="22"/>
+      <c r="CW2" s="22"/>
+      <c r="CX2" s="22"/>
     </row>
     <row r="3" spans="1:104" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>113</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1480,10 +1480,10 @@
       <c r="CX3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="CY3" s="24" t="s">
+      <c r="CY3" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="CZ3" s="22" t="s">
+      <c r="CZ3" s="20" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3125,10 +3125,10 @@
         <v>0.888378</v>
       </c>
       <c r="V9" s="16">
-        <v>0.81481729999999997</v>
+        <v>0.80264970000000002</v>
       </c>
       <c r="W9" s="16">
-        <v>0.88390009999999997</v>
+        <v>0.8785425</v>
       </c>
       <c r="X9" s="16">
         <v>0.84699519999999995</v>
@@ -3143,7 +3143,7 @@
         <v>0.91714660000000003</v>
       </c>
       <c r="AB9" s="16">
-        <v>0.81562939999999995</v>
+        <v>0.80692770000000003</v>
       </c>
       <c r="AC9" s="16">
         <v>0.87272910000000004</v>
@@ -3197,7 +3197,7 @@
         <v>0.78306880000000001</v>
       </c>
       <c r="AT9" s="16">
-        <v>0.85077670000000005</v>
+        <v>0.84352769999999999</v>
       </c>
       <c r="AU9" s="16">
         <v>0.85606059999999995</v>
@@ -3257,7 +3257,7 @@
         <v>0.73960029999999999</v>
       </c>
       <c r="BN9" s="16">
-        <v>0.8680523</v>
+        <v>0.86262629999999996</v>
       </c>
       <c r="BO9" s="16">
         <v>0.69195399999999996</v>
@@ -3272,7 +3272,7 @@
         <v>0.77615959999999995</v>
       </c>
       <c r="BS9" s="16">
-        <v>0.88249080000000002</v>
+        <v>0.87546310000000005</v>
       </c>
       <c r="BT9" s="16">
         <v>0.87616119999999997</v>
@@ -3332,7 +3332,7 @@
         <v>0.91087340000000006</v>
       </c>
       <c r="CM9" s="16">
-        <v>0.88035850000000004</v>
+        <v>0.87393399999999999</v>
       </c>
       <c r="CN9" s="16">
         <v>0.83372710000000005</v>
@@ -3365,11 +3365,11 @@
         <v>0.9331332</v>
       </c>
       <c r="CX9" s="16">
-        <v>0.89439860000000004</v>
+        <v>0.888378</v>
       </c>
       <c r="CY9" s="18">
         <f t="shared" si="0"/>
-        <v>0.86283738600000026</v>
+        <v>0.86225363900000018</v>
       </c>
       <c r="CZ9" s="7" t="s">
         <v>124</v>
@@ -3572,7 +3572,7 @@
         <v>0.90601030000000005</v>
       </c>
       <c r="BN10" s="16">
-        <v>0.85783370000000003</v>
+        <v>0.85194550000000002</v>
       </c>
       <c r="BO10" s="16">
         <v>0.77471259999999997</v>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="CY10" s="13">
         <f t="shared" si="0"/>
-        <v>0.8292016390000001</v>
+        <v>0.82914275700000006</v>
       </c>
       <c r="CZ10" s="7" t="s">
         <v>125</v>
@@ -3773,7 +3773,7 @@
         <v>0.24140900000000001</v>
       </c>
       <c r="AB11" s="16">
-        <v>0.55695600000000001</v>
+        <v>0.56446209999999997</v>
       </c>
       <c r="AC11" s="16">
         <v>0.21972939999999999</v>
@@ -3827,7 +3827,7 @@
         <v>4.6277400000000003E-2</v>
       </c>
       <c r="AT11" s="16">
-        <v>0.75577289999999997</v>
+        <v>0.75286410000000004</v>
       </c>
       <c r="AU11" s="16">
         <v>0.38014779999999998</v>
@@ -3887,7 +3887,7 @@
         <v>0.72375610000000001</v>
       </c>
       <c r="BN11" s="16">
-        <v>0.34703309999999998</v>
+        <v>0.35143619999999998</v>
       </c>
       <c r="BO11" s="16">
         <v>0.10945870000000001</v>
@@ -3999,7 +3999,7 @@
       </c>
       <c r="CY11" s="13">
         <f t="shared" si="0"/>
-        <v>0.29154337738000008</v>
+        <v>0.29163338138000006</v>
       </c>
       <c r="CZ11" s="7"/>
     </row>
@@ -4383,10 +4383,10 @@
         <v>0.62903229999999999</v>
       </c>
       <c r="V13" s="17">
-        <v>0.65018589999999998</v>
+        <v>0.62599470000000002</v>
       </c>
       <c r="W13" s="17">
-        <v>0.84028239999999998</v>
+        <v>0.83265860000000003</v>
       </c>
       <c r="X13" s="17">
         <v>0.64706189999999997</v>
@@ -4401,7 +4401,7 @@
         <v>0.71919770000000005</v>
       </c>
       <c r="AB13" s="17">
-        <v>0.70573920000000001</v>
+        <v>0.691469</v>
       </c>
       <c r="AC13" s="17">
         <v>0.73279349999999999</v>
@@ -4455,7 +4455,7 @@
         <v>0.74801320000000004</v>
       </c>
       <c r="AT13" s="17">
-        <v>0.688724</v>
+        <v>0.6728307</v>
       </c>
       <c r="AU13" s="17">
         <v>0.64015149999999998</v>
@@ -4515,7 +4515,7 @@
         <v>0.49306680000000003</v>
       </c>
       <c r="BN13" s="17">
-        <v>0.71214330000000003</v>
+        <v>0.69969700000000001</v>
       </c>
       <c r="BO13" s="17">
         <v>0.48443199999999997</v>
@@ -4530,7 +4530,7 @@
         <v>0.55511339999999998</v>
       </c>
       <c r="BS13" s="17">
-        <v>0.75663259999999999</v>
+        <v>0.74074070000000003</v>
       </c>
       <c r="BT13" s="17">
         <v>0.71103850000000002</v>
@@ -4590,7 +4590,7 @@
         <v>0.75757580000000002</v>
       </c>
       <c r="CM13" s="17">
-        <v>0.70777509999999999</v>
+        <v>0.69070209999999999</v>
       </c>
       <c r="CN13" s="17">
         <v>0.65509430000000002</v>
@@ -4623,11 +4623,11 @@
         <v>0.82794909999999999</v>
       </c>
       <c r="CX13" s="17">
-        <v>0.8272138</v>
+        <v>0.81660949999999999</v>
       </c>
       <c r="CY13" s="14">
         <f t="shared" si="0"/>
-        <v>0.68795127700000014</v>
+        <v>0.68677133700000015</v>
       </c>
       <c r="CZ13" s="9"/>
     </row>

</xml_diff>